<commit_message>
fredig med å fylle ut
</commit_message>
<xml_diff>
--- a/Resultater/Resultater.xlsx
+++ b/Resultater/Resultater.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="d4 400_24" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="4">
   <si>
     <t>Pressure</t>
   </si>
@@ -95,7 +95,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="nb-NO" baseline="0"/>
-              <a:t> one</a:t>
+              <a:t> one at 400 A</a:t>
             </a:r>
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
@@ -1246,7 +1246,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="nb-NO" baseline="0"/>
-              <a:t> one</a:t>
+              <a:t> two at 400 A</a:t>
             </a:r>
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
@@ -1845,7 +1845,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="nb-NO" baseline="0"/>
-              <a:t> one</a:t>
+              <a:t> one at 630</a:t>
             </a:r>
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
@@ -2503,6 +2503,695 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>Interruption test for geometry</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="nb-NO" baseline="0"/>
+              <a:t> two at 630 A</a:t>
+            </a:r>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1. CZ Faliure</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="44"/>
+            <c:marker>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:ln>
+              </c:spPr>
+            </c:marker>
+          </c:dPt>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$A$2:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1. CZ Success</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$B$20:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$A$20:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2. CZ Faliure</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$J$2:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$G$2:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2. CZ Success</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$J$13:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'d3 630_24'!$G$13:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="69875968"/>
+        <c:axId val="69886720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="69875968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="110"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:alpha val="25000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>possition in nozzle</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nb-NO" baseline="0"/>
+                  <a:t> for CZ [mm]</a:t>
+                </a:r>
+                <a:endParaRPr lang="nb-NO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69886720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="69886720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2.1"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Pressure difference</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="nb-NO" baseline="0"/>
+                  <a:t> [bar]</a:t>
+                </a:r>
+                <a:endParaRPr lang="nb-NO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="69875968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2586,6 +3275,41 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>130549</xdr:colOff>
       <xdr:row>81</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>435349</xdr:colOff>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6042,8 +6766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="V56" sqref="V56"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7063,12 +7787,1087 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>0.9</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>95</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.9</v>
+      </c>
+      <c r="H2">
+        <v>56</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>105</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>0.9</v>
+      </c>
+      <c r="B3">
+        <v>56</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>105</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>89</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>0.9</v>
+      </c>
+      <c r="B4">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>89</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.9</v>
+      </c>
+      <c r="H4">
+        <v>48</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>97</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>0.9</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>97</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0.9</v>
+      </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>97</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>0.9</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>105</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>37</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>85</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>0.9</v>
+      </c>
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>97</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>94</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>85</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>44</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>92</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>97</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>94</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>94</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>91</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>97</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>60</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B13">
+        <v>42</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>94</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.9</v>
+      </c>
+      <c r="H13">
+        <v>46</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>95</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B14">
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>94</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.9</v>
+      </c>
+      <c r="H14">
+        <v>56</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>105</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>91</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>90</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>1.2</v>
+      </c>
+      <c r="B16">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>93</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H16">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>94</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>1.3</v>
+      </c>
+      <c r="B17">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>92</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1.2</v>
+      </c>
+      <c r="H17">
+        <v>44</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>93</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1.3</v>
+      </c>
+      <c r="H18">
+        <v>43</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>92</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>58</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>49</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>49</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>36</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>44</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>50</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>46</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>0.9</v>
+      </c>
+      <c r="B25">
+        <v>53</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0.9</v>
+      </c>
+      <c r="H25">
+        <v>53</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>41</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B27">
+        <v>56</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H27">
+        <v>56</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B28">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H28">
+        <v>40</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>1.2</v>
+      </c>
+      <c r="B29">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1.2</v>
+      </c>
+      <c r="H29">
+        <v>31</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>1.2</v>
+      </c>
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1.2</v>
+      </c>
+      <c r="H30">
+        <v>35</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>1.2</v>
+      </c>
+      <c r="B31">
+        <v>41</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1.2</v>
+      </c>
+      <c r="H31">
+        <v>41</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>1.2</v>
+      </c>
+      <c r="B32">
+        <v>42</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1.2</v>
+      </c>
+      <c r="H32">
+        <v>42</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33">
+        <v>1.2</v>
+      </c>
+      <c r="B33">
+        <v>43</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1.2</v>
+      </c>
+      <c r="H33">
+        <v>43</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34">
+        <v>1.3</v>
+      </c>
+      <c r="B34">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1.3</v>
+      </c>
+      <c r="H34">
+        <v>41</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35">
+        <v>1.3</v>
+      </c>
+      <c r="B35">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1.3</v>
+      </c>
+      <c r="H35">
+        <v>40</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36">
+        <v>1.3</v>
+      </c>
+      <c r="B36">
+        <v>43</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1.3</v>
+      </c>
+      <c r="H36">
+        <v>43</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37">
+        <v>1.3</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1.3</v>
+      </c>
+      <c r="H37">
+        <v>45</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38">
+        <v>1.4</v>
+      </c>
+      <c r="B38">
+        <v>42</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>1.4</v>
+      </c>
+      <c r="H38">
+        <v>42</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39">
+        <v>1.4</v>
+      </c>
+      <c r="B39">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1.4</v>
+      </c>
+      <c r="H39">
+        <v>45</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40">
+        <v>1.4</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1.4</v>
+      </c>
+      <c r="H40">
+        <v>40</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41">
+        <v>1.4</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1.4</v>
+      </c>
+      <c r="H41">
+        <v>40</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42">
+        <v>1.4</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1.4</v>
+      </c>
+      <c r="H42">
+        <v>41</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="G2:K42">
+    <sortCondition ref="K2:K42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
før flytting av posisjon excel
</commit_message>
<xml_diff>
--- a/Resultater/Resultater.xlsx
+++ b/Resultater/Resultater.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="28515" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="d4 400_24" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="20">
   <si>
     <t>Pressure</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>Denne viser at når man kommer over et hvist trykk så bryter den like bra på 1. som 2. CZ, men den bryter ikke inni, derfor er det nyttig å ha med to nullgjennomganger.</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>one 630</t>
+  </si>
+  <si>
+    <t>one</t>
   </si>
 </sst>
 </file>
@@ -1148,11 +1157,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88827392"/>
-        <c:axId val="88829312"/>
+        <c:axId val="76422528"/>
+        <c:axId val="76445952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88827392"/>
+        <c:axId val="76422528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1205,13 +1214,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88829312"/>
+        <c:crossAx val="76445952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88829312"/>
+        <c:axId val="76445952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -1253,7 +1262,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88827392"/>
+        <c:crossAx val="76422528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1267,7 +1276,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1278,6 +1287,21 @@
   <c:lang val="nb-NO"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nb-NO"/>
+              <a:t>Interruption successrate</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -1290,6 +1314,26 @@
           <c:tx>
             <c:v>Total successrate</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'d4 400_24'!$V$60:$V$71</c:f>
@@ -1387,6 +1431,28 @@
           <c:tx>
             <c:v>1. CZ chance of interruption if outside nozzle</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:prstClr val="black"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'d4 400_24'!$V$60:$V$71</c:f>
@@ -1472,9 +1538,23 @@
           <c:tx>
             <c:v>2. CZ chance of interruption if first CZ failed</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
               <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
@@ -1525,28 +1605,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="89741184"/>
-        <c:axId val="90006272"/>
+        <c:axId val="76940416"/>
+        <c:axId val="76941952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89741184"/>
+        <c:axId val="76940416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90006272"/>
+        <c:crossAx val="76941952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90006272"/>
+        <c:axId val="76941952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1560,7 +1640,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89741184"/>
+        <c:crossAx val="76940416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1574,7 +1654,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2054,11 +2134,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="88383488"/>
-        <c:axId val="88385792"/>
+        <c:axId val="77182080"/>
+        <c:axId val="77184384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88383488"/>
+        <c:axId val="77182080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2127,13 +2207,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88385792"/>
+        <c:crossAx val="77184384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88385792"/>
+        <c:axId val="77184384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -2175,7 +2255,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88383488"/>
+        <c:crossAx val="77182080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2189,13 +2269,234 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Geometriy one 400</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d3 400_24'!$AA$13:$AA$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 400_24'!$AB$13:$AB$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.666666666666657</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.777777777777786</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.909090909090907</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Geometry two</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d3 400_24'!$AA$13:$AA$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 400_24'!$AC$13:$AC$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="86181760"/>
+        <c:axId val="86183296"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="86181760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86183296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="86183296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="86181760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="nb-NO"/>
   <c:chart>
@@ -2747,11 +3048,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="65986560"/>
-        <c:axId val="65988864"/>
+        <c:axId val="77380608"/>
+        <c:axId val="77399552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65986560"/>
+        <c:axId val="77380608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2820,13 +3121,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65988864"/>
+        <c:crossAx val="77399552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65988864"/>
+        <c:axId val="77399552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -2868,7 +3169,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65986560"/>
+        <c:crossAx val="77380608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2882,13 +3183,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000051" r="0.70000000000000051" t="0.78740157499999996" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="nb-NO"/>
   <c:chart>
@@ -3452,11 +3753,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69875968"/>
-        <c:axId val="69886720"/>
+        <c:axId val="77541760"/>
+        <c:axId val="77544064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69875968"/>
+        <c:axId val="77541760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -3525,13 +3826,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69886720"/>
+        <c:crossAx val="77544064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69886720"/>
+        <c:axId val="77544064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -3573,7 +3874,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69875968"/>
+        <c:crossAx val="77541760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3588,6 +3889,213 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Geometry two 630 A</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d4 630_24'!$T$4:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AG$21:$AG$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="2">
+                  <c:v>42.857142857142854</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Geometry one 630 A</c:v>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d4 630_24'!$T$4:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AH$21:$AH$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="96133888"/>
+        <c:axId val="96135424"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="96133888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96135424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96135424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="96133888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3690,6 +4198,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3755,6 +4293,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>324970</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4050,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView topLeftCell="F46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V59" sqref="V59:V71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5988,7 +6556,7 @@
         <v>0</v>
       </c>
       <c r="X60">
-        <f>W60/Y60*100</f>
+        <f t="shared" ref="X60:X71" si="0">W60/Y60*100</f>
         <v>0</v>
       </c>
       <c r="Y60">
@@ -6001,7 +6569,7 @@
         <v>3</v>
       </c>
       <c r="AB60">
-        <f>Z60/AA60*100</f>
+        <f t="shared" ref="AB60:AB71" si="1">Z60/AA60*100</f>
         <v>0</v>
       </c>
       <c r="AC60">
@@ -6052,7 +6620,7 @@
         <v>0</v>
       </c>
       <c r="X61">
-        <f>W61/Y61*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y61">
@@ -6065,7 +6633,7 @@
         <v>5</v>
       </c>
       <c r="AB61">
-        <f>Z61/AA61*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC61">
@@ -6116,7 +6684,7 @@
         <v>4</v>
       </c>
       <c r="X62">
-        <f>W62/Y62*100</f>
+        <f t="shared" si="0"/>
         <v>66.666666666666657</v>
       </c>
       <c r="Y62">
@@ -6129,7 +6697,7 @@
         <v>2</v>
       </c>
       <c r="AB62">
-        <f>Z62/AA62*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC62">
@@ -6181,7 +6749,7 @@
         <v>4</v>
       </c>
       <c r="X63">
-        <f>W63/Y63*100</f>
+        <f t="shared" si="0"/>
         <v>44.444444444444443</v>
       </c>
       <c r="Y63">
@@ -6194,14 +6762,14 @@
         <v>5</v>
       </c>
       <c r="AB63">
-        <f>Z63/AA63*100</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="AC63">
         <v>9</v>
       </c>
       <c r="AD63">
-        <f>(W63+Z63)/AC63*100</f>
+        <f t="shared" ref="AD63:AD71" si="2">(W63+Z63)/AC63*100</f>
         <v>77.777777777777786</v>
       </c>
     </row>
@@ -6246,7 +6814,7 @@
         <v>4</v>
       </c>
       <c r="X64">
-        <f>W64/Y64*100</f>
+        <f t="shared" si="0"/>
         <v>36.363636363636367</v>
       </c>
       <c r="Y64">
@@ -6259,14 +6827,14 @@
         <v>7</v>
       </c>
       <c r="AB64">
-        <f>Z64/AA64*100</f>
+        <f t="shared" si="1"/>
         <v>85.714285714285708</v>
       </c>
       <c r="AC64">
         <v>11</v>
       </c>
       <c r="AD64">
-        <f>(W64+Z64)/AC64*100</f>
+        <f t="shared" si="2"/>
         <v>90.909090909090907</v>
       </c>
     </row>
@@ -6311,7 +6879,7 @@
         <v>8</v>
       </c>
       <c r="X65">
-        <f>W65/Y65*100</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="Y65">
@@ -6324,14 +6892,14 @@
         <v>8</v>
       </c>
       <c r="AB65">
-        <f>Z65/AA65*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC65">
         <v>16</v>
       </c>
       <c r="AD65">
-        <f>(W65+Z65)/AC65*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6376,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="X66">
-        <f>W66/Y66*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y66">
@@ -6389,14 +6957,14 @@
         <v>2</v>
       </c>
       <c r="AB66">
-        <f>Z66/AA66*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC66">
         <v>2</v>
       </c>
       <c r="AD66">
-        <f>(W66+Z66)/AC66*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6441,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="X67">
-        <f>W67/Y67*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y67">
@@ -6454,14 +7022,14 @@
         <v>2</v>
       </c>
       <c r="AB67">
-        <f>Z67/AA67*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC67">
         <v>2</v>
       </c>
       <c r="AD67">
-        <f>(W67+Z67)/AC67*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6500,7 +7068,7 @@
         <v>0</v>
       </c>
       <c r="X68">
-        <f>W68/Y68*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y68">
@@ -6513,14 +7081,14 @@
         <v>2</v>
       </c>
       <c r="AB68">
-        <f>Z68/AA68*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC68">
         <v>2</v>
       </c>
       <c r="AD68">
-        <f>(W68+Z68)/AC68*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6559,7 +7127,7 @@
         <v>3</v>
       </c>
       <c r="X69">
-        <f>W69/Y69*100</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="Y69">
@@ -6572,14 +7140,14 @@
         <v>1</v>
       </c>
       <c r="AB69">
-        <f>Z69/AA69*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC69">
         <v>4</v>
       </c>
       <c r="AD69">
-        <f>(W69+Z69)/AC69*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6618,7 +7186,7 @@
         <v>0</v>
       </c>
       <c r="X70">
-        <f>W70/Y70*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y70">
@@ -6631,14 +7199,14 @@
         <v>1</v>
       </c>
       <c r="AB70">
-        <f>Z70/AA70*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AC70">
         <v>1</v>
       </c>
       <c r="AD70">
-        <f>(W70+Z70)/AC70*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -6683,7 +7251,7 @@
         <v>1</v>
       </c>
       <c r="X71">
-        <f>W71/Y71*100</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="Y71">
@@ -6696,14 +7264,14 @@
         <v>4</v>
       </c>
       <c r="AB71">
-        <f>Z71/AA71*100</f>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="AC71">
         <v>5</v>
       </c>
       <c r="AD71">
-        <f>(W71+Z71)/AC71*100</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
@@ -7001,7 +7569,7 @@
         <v>4</v>
       </c>
       <c r="AA78">
-        <f t="shared" ref="AA78:AA83" si="0">Y78/Z78*100</f>
+        <f t="shared" ref="AA78:AA82" si="3">Y78/Z78*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7049,7 +7617,7 @@
         <v>6</v>
       </c>
       <c r="AA79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>66.666666666666657</v>
       </c>
     </row>
@@ -7097,7 +7665,7 @@
         <v>5</v>
       </c>
       <c r="AA80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
@@ -7151,7 +7719,7 @@
         <v>5</v>
       </c>
       <c r="AA81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
     </row>
@@ -7199,7 +7767,7 @@
         <v>8</v>
       </c>
       <c r="AA82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -7367,7 +7935,7 @@
         <v>3</v>
       </c>
       <c r="AA86">
-        <f t="shared" ref="AA86:AA88" si="1">Y86/Z86*100</f>
+        <f t="shared" ref="AA86:AA88" si="4">Y86/Z86*100</f>
         <v>100</v>
       </c>
     </row>
@@ -7435,7 +8003,7 @@
         <v>1</v>
       </c>
       <c r="AA88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -7928,7 +8496,7 @@
         <v>72.5</v>
       </c>
       <c r="T122">
-        <f t="shared" ref="T122" si="2">R122/S122*100</f>
+        <f t="shared" ref="T122" si="5">R122/S122*100</f>
         <v>0</v>
       </c>
     </row>
@@ -7989,15 +8557,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8028,8 +8596,26 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2">
         <v>0.6</v>
       </c>
@@ -8060,8 +8646,29 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="O2">
+        <v>0.6</v>
+      </c>
+      <c r="P2">
+        <v>7.5</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>57.5</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3">
         <v>0.6</v>
       </c>
@@ -8092,8 +8699,50 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="O3">
+        <v>0.6</v>
+      </c>
+      <c r="P3">
+        <v>7.5</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>62.5</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
       <c r="A4">
         <v>0.6</v>
       </c>
@@ -8124,8 +8773,53 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+      <c r="P4">
+        <v>12.5</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>62.5</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0.6</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <f>W4/Y4*100</f>
+        <v>10</v>
+      </c>
+      <c r="Y4">
+        <v>10</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>9</v>
+      </c>
+      <c r="AB4">
+        <f>Z4/AA4*100</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="AC4">
+        <v>10</v>
+      </c>
+      <c r="AD4">
+        <f>(W4+Z4)/AC4*100</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
       <c r="A5">
         <v>0.6</v>
       </c>
@@ -8156,8 +8850,53 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="O5">
+        <v>0.6</v>
+      </c>
+      <c r="P5">
+        <v>17.5</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>72.5</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0.7</v>
+      </c>
+      <c r="W5">
+        <v>7</v>
+      </c>
+      <c r="X5">
+        <f>W5/Y5*100</f>
+        <v>87.5</v>
+      </c>
+      <c r="Y5">
+        <v>8</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <f>Z5/AA5*100</f>
+        <v>100</v>
+      </c>
+      <c r="AC5">
+        <v>8</v>
+      </c>
+      <c r="AD5">
+        <f>(W5+Z5)/AC5*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
       <c r="A6">
         <v>0.6</v>
       </c>
@@ -8188,8 +8927,53 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="O6">
+        <v>0.6</v>
+      </c>
+      <c r="P6">
+        <v>22.5</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>72.5</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f>W6/Y6*100</f>
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <f>Z6/AA6*100</f>
+        <v>100</v>
+      </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <f>(W6+Z6)/AC6*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
       <c r="A7">
         <v>0.6</v>
       </c>
@@ -8220,8 +9004,23 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="O7">
+        <v>0.6</v>
+      </c>
+      <c r="P7">
+        <v>37.5</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>90</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -8252,8 +9051,23 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="O8">
+        <v>0.6</v>
+      </c>
+      <c r="P8">
+        <v>37.5</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>90</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
       <c r="A9">
         <v>0.6</v>
       </c>
@@ -8284,8 +9098,23 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="O9">
+        <v>0.6</v>
+      </c>
+      <c r="P9">
+        <v>45</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>105</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
       <c r="A10">
         <v>0.6</v>
       </c>
@@ -8316,8 +9145,17 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="O10">
+        <v>0.6</v>
+      </c>
+      <c r="P10">
+        <v>52.5</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
       <c r="A11">
         <v>0.6</v>
       </c>
@@ -8348,8 +9186,23 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="O11">
+        <v>0.6</v>
+      </c>
+      <c r="P11">
+        <v>55</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>110</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -8380,8 +9233,29 @@
       <c r="K12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="O12">
+        <v>0.7</v>
+      </c>
+      <c r="P12">
+        <v>42.5</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>97.5</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
       <c r="A13">
         <v>0.6</v>
       </c>
@@ -8412,8 +9286,23 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="O13">
+        <v>0.7</v>
+      </c>
+      <c r="P13">
+        <v>42.5</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>0.3</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
       <c r="A14">
         <v>0.7</v>
       </c>
@@ -8444,8 +9333,23 @@
       <c r="K14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="O14">
+        <v>0.7</v>
+      </c>
+      <c r="P14">
+        <v>50</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>0.4</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
       <c r="A15">
         <v>2</v>
       </c>
@@ -8476,8 +9380,23 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="O15">
+        <v>0.7</v>
+      </c>
+      <c r="P15">
+        <v>50</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>0.5</v>
+      </c>
+      <c r="AB15">
+        <v>66.666666666666657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16">
         <v>2</v>
       </c>
@@ -8508,8 +9427,26 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="O16">
+        <v>0.7</v>
+      </c>
+      <c r="P16">
+        <v>52.5</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>0.6</v>
+      </c>
+      <c r="AB16">
+        <v>77.777777777777786</v>
+      </c>
+      <c r="AC16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>2</v>
       </c>
@@ -8540,8 +9477,26 @@
       <c r="K17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="O17">
+        <v>0.7</v>
+      </c>
+      <c r="P17">
+        <v>52.5</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>0.7</v>
+      </c>
+      <c r="AB17">
+        <v>90.909090909090907</v>
+      </c>
+      <c r="AC17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>2</v>
       </c>
@@ -8572,8 +9527,26 @@
       <c r="K18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="O18">
+        <v>0.7</v>
+      </c>
+      <c r="P18">
+        <v>52.5</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>0.8</v>
+      </c>
+      <c r="AB18">
+        <v>100</v>
+      </c>
+      <c r="AC18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>2</v>
       </c>
@@ -8604,8 +9577,23 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="O19">
+        <v>0.7</v>
+      </c>
+      <c r="P19">
+        <v>52.5</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>0.7</v>
       </c>
@@ -8624,8 +9612,29 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>17.5</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>77.5</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1.2</v>
+      </c>
+      <c r="AB20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>0.7</v>
       </c>
@@ -8644,8 +9653,29 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>22.5</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>82.5</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1.4</v>
+      </c>
+      <c r="AB21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>0.7</v>
       </c>
@@ -8664,8 +9694,14 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="AA22">
+        <v>1.6</v>
+      </c>
+      <c r="AB22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>0.7</v>
       </c>
@@ -8684,8 +9720,14 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="AA23">
+        <v>1.8</v>
+      </c>
+      <c r="AB23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>0.7</v>
       </c>
@@ -8704,8 +9746,14 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="AA24">
+        <v>2</v>
+      </c>
+      <c r="AB24">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>0.6</v>
       </c>
@@ -8725,7 +9773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:29">
       <c r="A26">
         <v>0.7</v>
       </c>
@@ -8745,7 +9793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:29">
       <c r="A27">
         <v>0.7</v>
       </c>
@@ -8766,8 +9814,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="G2:K27">
-    <sortCondition ref="K2:K27"/>
+  <sortState ref="O2:S27">
+    <sortCondition ref="O2:O27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8776,15 +9824,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="W68" sqref="W68"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8815,8 +9863,26 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2">
         <v>0.8</v>
       </c>
@@ -8847,8 +9913,29 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="O2">
+        <v>0.6</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>63</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3">
         <v>0.8</v>
       </c>
@@ -8879,8 +9966,50 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="O3">
+        <v>0.8</v>
+      </c>
+      <c r="P3">
+        <v>12</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>63</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
       <c r="A4">
         <v>0.8</v>
       </c>
@@ -8911,8 +10040,53 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="O4">
+        <v>0.8</v>
+      </c>
+      <c r="P4">
+        <v>35</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>82</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0.6</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f>U4/W4*100</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <f>X4/Y4*100</f>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <f>(U4+X4)/AA4*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
       <c r="A5">
         <v>0.8</v>
       </c>
@@ -8943,8 +10117,47 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="O5">
+        <v>0.8</v>
+      </c>
+      <c r="P5">
+        <v>35</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>0.8</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <f>U5/W5*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <f>X5/Y5*100</f>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>6</v>
+      </c>
+      <c r="AB5">
+        <f>(U5+X5)/AA5*100</f>
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
       <c r="A6">
         <v>0.8</v>
       </c>
@@ -8975,8 +10188,53 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="O6">
+        <v>0.8</v>
+      </c>
+      <c r="P6">
+        <v>40</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>88</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0.9</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <f>U6/W6*100</f>
+        <v>20</v>
+      </c>
+      <c r="W6">
+        <v>5</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <f>X6/Y6*100</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
+      <c r="AB6">
+        <f>(U6+X6)/AA6*100</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
       <c r="A7">
         <v>0.9</v>
       </c>
@@ -9007,8 +10265,53 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="O7">
+        <v>0.8</v>
+      </c>
+      <c r="P7">
+        <v>46</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>94</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <f>U7/W7*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="W7">
+        <v>6</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <f>X7/Y7*100</f>
+        <v>20</v>
+      </c>
+      <c r="AA7">
+        <v>5</v>
+      </c>
+      <c r="AB7">
+        <f>(U7+X7)/AA7*100</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
       <c r="A8">
         <v>0.9</v>
       </c>
@@ -9039,8 +10342,53 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="O8">
+        <v>0.8</v>
+      </c>
+      <c r="P8">
+        <v>55</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>102</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="U8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <f>U8/W8*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <f>X8/Y8*100</f>
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>6</v>
+      </c>
+      <c r="AB8">
+        <f>(U8+X8)/AA8*100</f>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
       <c r="A9">
         <v>0.9</v>
       </c>
@@ -9071,8 +10419,53 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="O9">
+        <v>0.9</v>
+      </c>
+      <c r="P9">
+        <v>45</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>95</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1.2</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <f>U9/W9*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="W9">
+        <v>6</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <f>X9/Y9*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <f>(U9+X9)/AA9*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
       <c r="A10">
         <v>0.9</v>
       </c>
@@ -9103,8 +10496,53 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="O10">
+        <v>0.9</v>
+      </c>
+      <c r="P10">
+        <v>49</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>98</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1.4</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f>U10/W10*100</f>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <f>X10/Y10*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <f>(U10+X10)/AA10*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
       <c r="A11">
         <v>0.9</v>
       </c>
@@ -9135,8 +10573,53 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="O11">
+        <v>0.9</v>
+      </c>
+      <c r="P11">
+        <v>50</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>98</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1.8</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <f>U11/W11*100</f>
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <f>X11/Y11*100</f>
+        <v>100</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <f>(U11+X11)/AA11*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
       <c r="A12">
         <v>1</v>
       </c>
@@ -9167,8 +10650,47 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="O12">
+        <v>0.9</v>
+      </c>
+      <c r="P12">
+        <v>50</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>2</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f>U12/W12*100</f>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <f>X12/Y12*100</f>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <f>(U12+X12)/AA12*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28">
       <c r="A13">
         <v>1</v>
       </c>
@@ -9199,8 +10721,23 @@
       <c r="K13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="O13">
+        <v>0.9</v>
+      </c>
+      <c r="P13">
+        <v>54</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>100</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
       <c r="A14">
         <v>1</v>
       </c>
@@ -9231,8 +10768,23 @@
       <c r="K14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>67</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28">
       <c r="A15">
         <v>1</v>
       </c>
@@ -9263,8 +10815,17 @@
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>42</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28">
       <c r="A16">
         <v>1.1000000000000001</v>
       </c>
@@ -9295,8 +10856,23 @@
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>43</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>91</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17">
         <v>1.2</v>
       </c>
@@ -9327,8 +10903,23 @@
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>44</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>92</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>1</v>
       </c>
@@ -9359,8 +10950,23 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>47</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>96</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>0.6</v>
       </c>
@@ -9391,8 +10997,23 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>51</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>97</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>1.4</v>
       </c>
@@ -9423,8 +11044,17 @@
       <c r="K20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="O20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P20">
+        <v>45</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>1.8</v>
       </c>
@@ -9455,8 +11085,23 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="O21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P21">
+        <v>48</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>97</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>2</v>
       </c>
@@ -9487,8 +11132,17 @@
       <c r="K22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="O22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P22">
+        <v>48</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>0.8</v>
       </c>
@@ -9507,8 +11161,17 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="O23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P23">
+        <v>53</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>0.9</v>
       </c>
@@ -9527,8 +11190,17 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="O24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P24">
+        <v>54</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>0.9</v>
       </c>
@@ -9547,8 +11219,17 @@
       <c r="I25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="O25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P25">
+        <v>56</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>1</v>
       </c>
@@ -9567,8 +11248,23 @@
       <c r="I26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="O26">
+        <v>1.2</v>
+      </c>
+      <c r="P26">
+        <v>13</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>68</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>1.1000000000000001</v>
       </c>
@@ -9587,8 +11283,17 @@
       <c r="I27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="O27">
+        <v>1.2</v>
+      </c>
+      <c r="P27">
+        <v>44</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>1.1000000000000001</v>
       </c>
@@ -9607,8 +11312,17 @@
       <c r="I28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="O28">
+        <v>1.2</v>
+      </c>
+      <c r="P28">
+        <v>44</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>1.1000000000000001</v>
       </c>
@@ -9627,8 +11341,17 @@
       <c r="I29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="O29">
+        <v>1.2</v>
+      </c>
+      <c r="P29">
+        <v>48</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>1.1000000000000001</v>
       </c>
@@ -9647,8 +11370,17 @@
       <c r="I30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="O30">
+        <v>1.2</v>
+      </c>
+      <c r="P30">
+        <v>51</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>1.1000000000000001</v>
       </c>
@@ -9667,8 +11399,17 @@
       <c r="I31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="O31">
+        <v>1.2</v>
+      </c>
+      <c r="P31">
+        <v>52</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>1.1000000000000001</v>
       </c>
@@ -9687,8 +11428,23 @@
       <c r="I32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="O32">
+        <v>1.4</v>
+      </c>
+      <c r="P32">
+        <v>20</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>73</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>1.2</v>
       </c>
@@ -9707,8 +11463,23 @@
       <c r="I33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="O33">
+        <v>1.8</v>
+      </c>
+      <c r="P33">
+        <v>13</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>68</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>1.2</v>
       </c>
@@ -9727,8 +11498,23 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="O34">
+        <v>2</v>
+      </c>
+      <c r="P34">
+        <v>16</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>70</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>1.2</v>
       </c>
@@ -9748,7 +11534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>1.2</v>
       </c>
@@ -9768,7 +11554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>1.2</v>
       </c>
@@ -9789,8 +11575,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="G2:K37">
-    <sortCondition ref="K2:K37"/>
+  <sortState ref="O2:S37">
+    <sortCondition ref="O2:O37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9799,15 +11585,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AG40" sqref="AG40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9838,8 +11624,29 @@
       <c r="K1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2">
         <v>0.9</v>
       </c>
@@ -9870,8 +11677,35 @@
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="O2">
+        <v>0.9</v>
+      </c>
+      <c r="P2">
+        <v>37</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>89</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
       <c r="A3">
         <v>0.9</v>
       </c>
@@ -9902,8 +11736,77 @@
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="O3">
+        <v>0.9</v>
+      </c>
+      <c r="P3">
+        <v>45</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>97</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
       <c r="A4">
         <v>0.9</v>
       </c>
@@ -9934,8 +11837,83 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="O4">
+        <v>0.9</v>
+      </c>
+      <c r="P4">
+        <v>46</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>95</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>0.9</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <f>W4/Y4*100</f>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="Y4">
+        <v>7</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>6</v>
+      </c>
+      <c r="AB4">
+        <f>Z4/AA4*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="AC4">
+        <v>7</v>
+      </c>
+      <c r="AD4">
+        <f>(W4+Z4)/AC4*100</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="AF4">
+        <v>0.6</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <f>AG4/AI4*100</f>
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <f>AJ4/AK4*100</f>
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <f>(AG4+AJ4)/AM4*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
       <c r="A5">
         <v>0.9</v>
       </c>
@@ -9966,8 +11944,83 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="O5">
+        <v>0.9</v>
+      </c>
+      <c r="P5">
+        <v>48</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>97</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>6</v>
+      </c>
+      <c r="X5">
+        <f>W5/Y5*100</f>
+        <v>60</v>
+      </c>
+      <c r="Y5">
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <f>Z5/AA5*100</f>
+        <v>25</v>
+      </c>
+      <c r="AC5">
+        <v>10</v>
+      </c>
+      <c r="AD5">
+        <f>(W5+Z5)/AC5*100</f>
+        <v>70</v>
+      </c>
+      <c r="AF5">
+        <v>0.8</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <f>AG5/AI5*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="AI5">
+        <v>6</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>5</v>
+      </c>
+      <c r="AL5">
+        <f>AJ5/AK5*100</f>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>6</v>
+      </c>
+      <c r="AN5">
+        <f>(AG5+AJ5)/AM5*100</f>
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
       <c r="A6">
         <v>0.9</v>
       </c>
@@ -9998,8 +12051,77 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="O6">
+        <v>0.9</v>
+      </c>
+      <c r="P6">
+        <v>53</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <f>W6/Y6*100</f>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="Y6">
+        <v>6</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
+      </c>
+      <c r="AB6">
+        <f>Z6/AA6*100</f>
+        <v>25</v>
+      </c>
+      <c r="AC6">
+        <v>6</v>
+      </c>
+      <c r="AD6">
+        <f>(W6+Z6)/AC6*100</f>
+        <v>50</v>
+      </c>
+      <c r="AF6">
+        <v>0.9</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <f>AG6/AI6*100</f>
+        <v>20</v>
+      </c>
+      <c r="AI6">
+        <v>5</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>4</v>
+      </c>
+      <c r="AL6">
+        <f>AJ6/AK6*100</f>
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>5</v>
+      </c>
+      <c r="AN6">
+        <f>(AG6+AJ6)/AM6*100</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
       <c r="A7">
         <v>0.9</v>
       </c>
@@ -10030,8 +12152,83 @@
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="O7">
+        <v>0.9</v>
+      </c>
+      <c r="P7">
+        <v>56</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>105</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>1.2</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <f>W7/Y7*100</f>
+        <v>80</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <f>Z7/AA7*100</f>
+        <v>100</v>
+      </c>
+      <c r="AC7">
+        <v>5</v>
+      </c>
+      <c r="AD7">
+        <f>(W7+Z7)/AC7*100</f>
+        <v>100</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <f>AG7/AI7*100</f>
+        <v>16.666666666666664</v>
+      </c>
+      <c r="AI7">
+        <v>6</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>5</v>
+      </c>
+      <c r="AL7">
+        <f>AJ7/AK7*100</f>
+        <v>20</v>
+      </c>
+      <c r="AM7">
+        <v>5</v>
+      </c>
+      <c r="AN7">
+        <f>(AG7+AJ7)/AM7*100</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
       <c r="A8">
         <v>1</v>
       </c>
@@ -10062,8 +12259,83 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="O8">
+        <v>0.9</v>
+      </c>
+      <c r="P8">
+        <v>56</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>105</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1.3</v>
+      </c>
+      <c r="W8">
+        <v>4</v>
+      </c>
+      <c r="X8">
+        <f>W8/Y8*100</f>
+        <v>80</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <f>Z8/AA8*100</f>
+        <v>100</v>
+      </c>
+      <c r="AC8">
+        <v>5</v>
+      </c>
+      <c r="AD8">
+        <f>(W8+Z8)/AC8*100</f>
+        <v>100</v>
+      </c>
+      <c r="AF8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AG8">
+        <v>5</v>
+      </c>
+      <c r="AH8">
+        <f>AG8/AI8*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="AI8">
+        <v>6</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <f>AJ8/AK8*100</f>
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>6</v>
+      </c>
+      <c r="AN8">
+        <f>(AG8+AJ8)/AM8*100</f>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
       <c r="A9">
         <v>1</v>
       </c>
@@ -10094,8 +12366,67 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>36</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1.4</v>
+      </c>
+      <c r="W9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <f>W9/Y9*100</f>
+        <v>100</v>
+      </c>
+      <c r="Y9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>5</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" ref="AD9:AD10" si="0">(W9+Z9)/AC9*100</f>
+        <v>100</v>
+      </c>
+      <c r="AF9">
+        <v>1.2</v>
+      </c>
+      <c r="AG9">
+        <v>5</v>
+      </c>
+      <c r="AH9">
+        <f>AG9/AI9*100</f>
+        <v>83.333333333333343</v>
+      </c>
+      <c r="AI9">
+        <v>6</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <f>AJ9/AK9*100</f>
+        <v>100</v>
+      </c>
+      <c r="AM9">
+        <v>6</v>
+      </c>
+      <c r="AN9">
+        <f>(AG9+AJ9)/AM9*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
       <c r="A10">
         <v>1</v>
       </c>
@@ -10126,8 +12457,83 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>37</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>85</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>2</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <f>W10/Y10*100</f>
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" ref="AB9:AB10" si="1">Z10/AA10*100</f>
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>1.4</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <f>AG10/AI10*100</f>
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <f>AJ10/AK10*100</f>
+        <v>100</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <f>(AG10+AJ10)/AM10*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
       <c r="A11">
         <v>1</v>
       </c>
@@ -10158,8 +12564,47 @@
       <c r="K11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>41</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1.8</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <f>AG11/AI11*100</f>
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <f>AJ11/AK11*100</f>
+        <v>100</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AN11">
+        <f>(AG11+AJ11)/AM11*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40">
       <c r="A12">
         <v>1.1000000000000001</v>
       </c>
@@ -10190,8 +12635,53 @@
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>42</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>90</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f>AG12/AI12*100</f>
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <f>AJ12/AK12*100</f>
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>1</v>
+      </c>
+      <c r="AN12">
+        <f>(AG12+AJ12)/AM12*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40">
       <c r="A13">
         <v>1.1000000000000001</v>
       </c>
@@ -10222,8 +12712,23 @@
       <c r="K13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>44</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>92</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40">
       <c r="A14">
         <v>1.1000000000000001</v>
       </c>
@@ -10254,8 +12759,17 @@
       <c r="K14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>44</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40">
       <c r="A15">
         <v>1.1000000000000001</v>
       </c>
@@ -10286,8 +12800,23 @@
       <c r="K15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>46</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>94</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40">
       <c r="A16">
         <v>1.2</v>
       </c>
@@ -10318,8 +12847,17 @@
       <c r="K16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>46</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34">
       <c r="A17">
         <v>1.3</v>
       </c>
@@ -10350,8 +12888,17 @@
       <c r="K17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>49</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34">
       <c r="A18">
         <v>2</v>
       </c>
@@ -10382,8 +12929,17 @@
       <c r="K18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>50</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34">
       <c r="A19">
         <v>2</v>
       </c>
@@ -10414,8 +12970,23 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="O19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P19">
+        <v>40</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>91</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34">
       <c r="A20">
         <v>1</v>
       </c>
@@ -10434,8 +13005,26 @@
       <c r="I20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="O20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P20">
+        <v>40</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34">
       <c r="A21">
         <v>1</v>
       </c>
@@ -10454,8 +13043,29 @@
       <c r="I21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="O21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P21">
+        <v>42</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>94</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0.6</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34">
       <c r="A22">
         <v>1</v>
       </c>
@@ -10474,8 +13084,29 @@
       <c r="I22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="O22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P22">
+        <v>42</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>94</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="AF22">
+        <v>0.8</v>
+      </c>
+      <c r="AH22">
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34">
       <c r="A23">
         <v>1</v>
       </c>
@@ -10494,8 +13125,32 @@
       <c r="I23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="O23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P23">
+        <v>45</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>97</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0.9</v>
+      </c>
+      <c r="AG23">
+        <v>42.857142857142854</v>
+      </c>
+      <c r="AH23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34">
       <c r="A24">
         <v>1</v>
       </c>
@@ -10514,8 +13169,26 @@
       <c r="I24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="O24">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P24">
+        <v>56</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>70</v>
+      </c>
+      <c r="AH24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34">
       <c r="A25">
         <v>0.9</v>
       </c>
@@ -10534,8 +13207,26 @@
       <c r="I25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="O25">
+        <v>1.2</v>
+      </c>
+      <c r="P25">
+        <v>35</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AG25">
+        <v>50</v>
+      </c>
+      <c r="AH25">
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34">
       <c r="A26">
         <v>1</v>
       </c>
@@ -10554,8 +13245,26 @@
       <c r="I26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="O26">
+        <v>1.2</v>
+      </c>
+      <c r="P26">
+        <v>41</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="AF26">
+        <v>1.2</v>
+      </c>
+      <c r="AG26">
+        <v>100</v>
+      </c>
+      <c r="AH26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34">
       <c r="A27">
         <v>1.1000000000000001</v>
       </c>
@@ -10574,8 +13283,26 @@
       <c r="I27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="O27">
+        <v>1.2</v>
+      </c>
+      <c r="P27">
+        <v>42</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>1.4</v>
+      </c>
+      <c r="AG27">
+        <v>100</v>
+      </c>
+      <c r="AH27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34">
       <c r="A28">
         <v>1.1000000000000001</v>
       </c>
@@ -10594,8 +13321,26 @@
       <c r="I28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="O28">
+        <v>1.2</v>
+      </c>
+      <c r="P28">
+        <v>43</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="AF28">
+        <v>1.8</v>
+      </c>
+      <c r="AG28">
+        <v>100</v>
+      </c>
+      <c r="AH28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34">
       <c r="A29">
         <v>1.2</v>
       </c>
@@ -10614,8 +13359,32 @@
       <c r="I29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="O29">
+        <v>1.2</v>
+      </c>
+      <c r="P29">
+        <v>44</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <v>93</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="AF29">
+        <v>2</v>
+      </c>
+      <c r="AG29">
+        <v>0</v>
+      </c>
+      <c r="AH29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34">
       <c r="A30">
         <v>1.2</v>
       </c>
@@ -10634,8 +13403,17 @@
       <c r="I30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="O30">
+        <v>1.3</v>
+      </c>
+      <c r="P30">
+        <v>40</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34">
       <c r="A31">
         <v>1.2</v>
       </c>
@@ -10654,8 +13432,17 @@
       <c r="I31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="O31">
+        <v>1.3</v>
+      </c>
+      <c r="P31">
+        <v>41</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34">
       <c r="A32">
         <v>1.2</v>
       </c>
@@ -10674,8 +13461,23 @@
       <c r="I32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="O32">
+        <v>1.3</v>
+      </c>
+      <c r="P32">
+        <v>43</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>92</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33">
         <v>1.2</v>
       </c>
@@ -10694,8 +13496,17 @@
       <c r="I33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="O33">
+        <v>1.3</v>
+      </c>
+      <c r="P33">
+        <v>43</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34">
         <v>1.3</v>
       </c>
@@ -10714,8 +13525,17 @@
       <c r="I34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="O34">
+        <v>1.3</v>
+      </c>
+      <c r="P34">
+        <v>45</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35">
         <v>1.3</v>
       </c>
@@ -10734,8 +13554,17 @@
       <c r="I35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="O35">
+        <v>1.4</v>
+      </c>
+      <c r="P35">
+        <v>40</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36">
         <v>1.3</v>
       </c>
@@ -10754,8 +13583,17 @@
       <c r="I36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="O36">
+        <v>1.4</v>
+      </c>
+      <c r="P36">
+        <v>40</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37">
         <v>1.3</v>
       </c>
@@ -10774,8 +13612,17 @@
       <c r="I37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="O37">
+        <v>1.4</v>
+      </c>
+      <c r="P37">
+        <v>41</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38">
         <v>1.4</v>
       </c>
@@ -10794,8 +13641,17 @@
       <c r="I38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="O38">
+        <v>1.4</v>
+      </c>
+      <c r="P38">
+        <v>42</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39">
         <v>1.4</v>
       </c>
@@ -10814,8 +13670,17 @@
       <c r="I39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:9">
+      <c r="O39">
+        <v>1.4</v>
+      </c>
+      <c r="P39">
+        <v>45</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40">
         <v>1.4</v>
       </c>
@@ -10834,8 +13699,23 @@
       <c r="I40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="O40">
+        <v>2</v>
+      </c>
+      <c r="P40">
+        <v>11</v>
+      </c>
+      <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <v>60</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41">
         <v>1.4</v>
       </c>
@@ -10855,7 +13735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:19">
       <c r="A42">
         <v>1.4</v>
       </c>
@@ -10876,8 +13756,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="G2:K42">
-    <sortCondition ref="K2:K42"/>
+  <sortState ref="O2:S42">
+    <sortCondition ref="O2:O42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
resultater er oppdatert for successrate bilder
</commit_message>
<xml_diff>
--- a/Resultater/Resultater.xlsx
+++ b/Resultater/Resultater.xlsx
@@ -150,7 +150,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1157,11 +1156,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76422528"/>
-        <c:axId val="76445952"/>
+        <c:axId val="87854464"/>
+        <c:axId val="87877888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76422528"/>
+        <c:axId val="87854464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -1209,18 +1208,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76445952"/>
+        <c:crossAx val="87877888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76445952"/>
+        <c:axId val="87877888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -1257,12 +1255,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76422528"/>
+        <c:crossAx val="87854464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1270,7 +1267,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1302,7 +1298,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1606,11 +1601,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76940416"/>
-        <c:axId val="76941952"/>
+        <c:axId val="87514496"/>
+        <c:axId val="87537152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76940416"/>
+        <c:axId val="87514496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,14 +1614,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76941952"/>
+        <c:crossAx val="87537152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76941952"/>
+        <c:axId val="87537152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,21 +1635,20 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="76940416"/>
+        <c:crossAx val="87514496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000029" r="0.70000000000000029" t="0.78740157499999996" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2134,11 +2128,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77182080"/>
-        <c:axId val="77184384"/>
+        <c:axId val="88145920"/>
+        <c:axId val="88148224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77182080"/>
+        <c:axId val="88145920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2207,13 +2201,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77184384"/>
+        <c:crossAx val="88148224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77184384"/>
+        <c:axId val="88148224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -2255,7 +2249,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77182080"/>
+        <c:crossAx val="88145920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2269,7 +2263,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2287,8 +2281,30 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Geometriy one 400</c:v>
+            <c:v>Geometry a, 400 A</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'d3 400_24'!$AA$13:$AA$24</c:f>
@@ -2384,8 +2400,30 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Geometry two</c:v>
+            <c:v>Geometry b, 400 A</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'d3 400_24'!$AA$13:$AA$24</c:f>
@@ -2451,35 +2489,80 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="86181760"/>
-        <c:axId val="86183296"/>
+        <c:axId val="88185472"/>
+        <c:axId val="88187648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86181760"/>
+        <c:axId val="88185472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Upstream over-pressure [bar]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86183296"/>
+        <c:crossAx val="88187648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86183296"/>
+        <c:axId val="88187648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Successful interruptions [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86181760"/>
-        <c:crosses val="autoZero"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="88185472"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2488,9 +2571,17 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2521,7 +2612,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3048,11 +3138,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77380608"/>
-        <c:axId val="77399552"/>
+        <c:axId val="88251776"/>
+        <c:axId val="88266624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77380608"/>
+        <c:axId val="88251776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -3116,18 +3206,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77399552"/>
+        <c:crossAx val="88266624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77399552"/>
+        <c:axId val="88266624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -3164,12 +3253,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77380608"/>
+        <c:crossAx val="88251776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3177,7 +3265,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3753,11 +3840,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77541760"/>
-        <c:axId val="77544064"/>
+        <c:axId val="88429312"/>
+        <c:axId val="88431616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77541760"/>
+        <c:axId val="88429312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -3826,13 +3913,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77544064"/>
+        <c:crossAx val="88431616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77544064"/>
+        <c:axId val="88431616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.1"/>
@@ -3874,7 +3961,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77541760"/>
+        <c:crossAx val="88429312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4055,25 +4142,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96133888"/>
-        <c:axId val="96135424"/>
+        <c:axId val="88415232"/>
+        <c:axId val="88462080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96133888"/>
+        <c:axId val="88415232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96135424"/>
+        <c:crossAx val="88462080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96135424"/>
+        <c:axId val="88462080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4081,7 +4168,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96133888"/>
+        <c:crossAx val="88415232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4095,7 +4182,310 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="nb-NO"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Geometry a, 630 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AF$21:$AF$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AH$21:$AH$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Geometry b, 630 A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AF$21:$AF$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d3 630_24'!$AG$21:$AG$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="2">
+                  <c:v>42.857142857142854</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="103347328"/>
+        <c:axId val="103349632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="103347328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Upstream over-pressure [bar]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="103349632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="103349632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Successful interruptions [%]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="103347328"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4200,16 +4590,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>472106</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>183046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>215347</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4323,6 +4713,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>459442</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>537882</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagram 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4618,7 +5038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF125"/>
   <sheetViews>
-    <sheetView topLeftCell="F19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C45" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
@@ -8556,8 +8976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="O2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Y50" sqref="Y50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9815,7 +10235,8 @@
     <sortCondition ref="O2:O27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10059,7 +10480,7 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <f>U4/W4*100</f>
+        <f t="shared" ref="V4:V12" si="0">U4/W4*100</f>
         <v>0</v>
       </c>
       <c r="W4">
@@ -10072,14 +10493,14 @@
         <v>1</v>
       </c>
       <c r="Z4">
-        <f>X4/Y4*100</f>
+        <f t="shared" ref="Z4:Z12" si="1">X4/Y4*100</f>
         <v>0</v>
       </c>
       <c r="AA4">
         <v>1</v>
       </c>
       <c r="AB4">
-        <f>(U4+X4)/AA4*100</f>
+        <f t="shared" ref="AB4:AB12" si="2">(U4+X4)/AA4*100</f>
         <v>0</v>
       </c>
     </row>
@@ -10130,7 +10551,7 @@
         <v>1</v>
       </c>
       <c r="V5">
-        <f>U5/W5*100</f>
+        <f t="shared" si="0"/>
         <v>16.666666666666664</v>
       </c>
       <c r="W5">
@@ -10143,14 +10564,14 @@
         <v>5</v>
       </c>
       <c r="Z5">
-        <f>X5/Y5*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA5">
         <v>6</v>
       </c>
       <c r="AB5">
-        <f>(U5+X5)/AA5*100</f>
+        <f t="shared" si="2"/>
         <v>16.666666666666664</v>
       </c>
     </row>
@@ -10207,7 +10628,7 @@
         <v>1</v>
       </c>
       <c r="V6">
-        <f>U6/W6*100</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="W6">
@@ -10220,14 +10641,14 @@
         <v>4</v>
       </c>
       <c r="Z6">
-        <f>X6/Y6*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA6">
         <v>5</v>
       </c>
       <c r="AB6">
-        <f>(U6+X6)/AA6*100</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -10284,7 +10705,7 @@
         <v>1</v>
       </c>
       <c r="V7">
-        <f>U7/W7*100</f>
+        <f t="shared" si="0"/>
         <v>16.666666666666664</v>
       </c>
       <c r="W7">
@@ -10297,14 +10718,14 @@
         <v>5</v>
       </c>
       <c r="Z7">
-        <f>X7/Y7*100</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AA7">
         <v>5</v>
       </c>
       <c r="AB7">
-        <f>(U7+X7)/AA7*100</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
@@ -10361,7 +10782,7 @@
         <v>5</v>
       </c>
       <c r="V8">
-        <f>U8/W8*100</f>
+        <f t="shared" si="0"/>
         <v>83.333333333333343</v>
       </c>
       <c r="W8">
@@ -10374,14 +10795,14 @@
         <v>1</v>
       </c>
       <c r="Z8">
-        <f>X8/Y8*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA8">
         <v>6</v>
       </c>
       <c r="AB8">
-        <f>(U8+X8)/AA8*100</f>
+        <f t="shared" si="2"/>
         <v>83.333333333333343</v>
       </c>
     </row>
@@ -10438,7 +10859,7 @@
         <v>5</v>
       </c>
       <c r="V9">
-        <f>U9/W9*100</f>
+        <f t="shared" si="0"/>
         <v>83.333333333333343</v>
       </c>
       <c r="W9">
@@ -10451,14 +10872,14 @@
         <v>1</v>
       </c>
       <c r="Z9">
-        <f>X9/Y9*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AA9">
         <v>6</v>
       </c>
       <c r="AB9">
-        <f>(U9+X9)/AA9*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -10515,7 +10936,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <f>U10/W10*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W10">
@@ -10528,14 +10949,14 @@
         <v>1</v>
       </c>
       <c r="Z10">
-        <f>X10/Y10*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AA10">
         <v>1</v>
       </c>
       <c r="AB10">
-        <f>(U10+X10)/AA10*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -10592,7 +11013,7 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <f>U11/W11*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W11">
@@ -10605,14 +11026,14 @@
         <v>1</v>
       </c>
       <c r="Z11">
-        <f>X11/Y11*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="AA11">
         <v>1</v>
       </c>
       <c r="AB11">
-        <f>(U11+X11)/AA11*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -10663,7 +11084,7 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <f>U12/W12*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="W12">
@@ -10676,14 +11097,14 @@
         <v>1</v>
       </c>
       <c r="Z12">
-        <f>X12/Y12*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA12">
         <v>1</v>
       </c>
       <c r="AB12">
-        <f>(U12+X12)/AA12*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -11584,8 +12005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="U37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL79" sqref="AL79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11856,7 +12277,7 @@
         <v>1</v>
       </c>
       <c r="X4">
-        <f>W4/Y4*100</f>
+        <f t="shared" ref="X4:X10" si="0">W4/Y4*100</f>
         <v>14.285714285714285</v>
       </c>
       <c r="Y4">
@@ -11886,7 +12307,7 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <f>AG4/AI4*100</f>
+        <f t="shared" ref="AH4:AH12" si="1">AG4/AI4*100</f>
         <v>0</v>
       </c>
       <c r="AI4">
@@ -11899,14 +12320,14 @@
         <v>1</v>
       </c>
       <c r="AL4">
-        <f>AJ4/AK4*100</f>
+        <f t="shared" ref="AL4:AL12" si="2">AJ4/AK4*100</f>
         <v>0</v>
       </c>
       <c r="AM4">
         <v>1</v>
       </c>
       <c r="AN4">
-        <f>(AG4+AJ4)/AM4*100</f>
+        <f t="shared" ref="AN4:AN12" si="3">(AG4+AJ4)/AM4*100</f>
         <v>0</v>
       </c>
     </row>
@@ -11963,7 +12384,7 @@
         <v>6</v>
       </c>
       <c r="X5">
-        <f>W5/Y5*100</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="Y5">
@@ -11993,7 +12414,7 @@
         <v>1</v>
       </c>
       <c r="AH5">
-        <f>AG5/AI5*100</f>
+        <f t="shared" si="1"/>
         <v>16.666666666666664</v>
       </c>
       <c r="AI5">
@@ -12006,14 +12427,14 @@
         <v>5</v>
       </c>
       <c r="AL5">
-        <f>AJ5/AK5*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM5">
         <v>6</v>
       </c>
       <c r="AN5">
-        <f>(AG5+AJ5)/AM5*100</f>
+        <f t="shared" si="3"/>
         <v>16.666666666666664</v>
       </c>
     </row>
@@ -12064,7 +12485,7 @@
         <v>2</v>
       </c>
       <c r="X6">
-        <f>W6/Y6*100</f>
+        <f t="shared" si="0"/>
         <v>33.333333333333329</v>
       </c>
       <c r="Y6">
@@ -12094,7 +12515,7 @@
         <v>1</v>
       </c>
       <c r="AH6">
-        <f>AG6/AI6*100</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="AI6">
@@ -12107,14 +12528,14 @@
         <v>4</v>
       </c>
       <c r="AL6">
-        <f>AJ6/AK6*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM6">
         <v>5</v>
       </c>
       <c r="AN6">
-        <f>(AG6+AJ6)/AM6*100</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
@@ -12171,7 +12592,7 @@
         <v>4</v>
       </c>
       <c r="X7">
-        <f>W7/Y7*100</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="Y7">
@@ -12201,7 +12622,7 @@
         <v>1</v>
       </c>
       <c r="AH7">
-        <f>AG7/AI7*100</f>
+        <f t="shared" si="1"/>
         <v>16.666666666666664</v>
       </c>
       <c r="AI7">
@@ -12214,14 +12635,14 @@
         <v>5</v>
       </c>
       <c r="AL7">
-        <f>AJ7/AK7*100</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AM7">
         <v>5</v>
       </c>
       <c r="AN7">
-        <f>(AG7+AJ7)/AM7*100</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
@@ -12278,7 +12699,7 @@
         <v>4</v>
       </c>
       <c r="X8">
-        <f>W8/Y8*100</f>
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="Y8">
@@ -12308,7 +12729,7 @@
         <v>5</v>
       </c>
       <c r="AH8">
-        <f>AG8/AI8*100</f>
+        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="AI8">
@@ -12321,14 +12742,14 @@
         <v>1</v>
       </c>
       <c r="AL8">
-        <f>AJ8/AK8*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM8">
         <v>6</v>
       </c>
       <c r="AN8">
-        <f>(AG8+AJ8)/AM8*100</f>
+        <f t="shared" si="3"/>
         <v>83.333333333333343</v>
       </c>
     </row>
@@ -12379,7 +12800,7 @@
         <v>5</v>
       </c>
       <c r="X9">
-        <f>W9/Y9*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="Y9">
@@ -12389,7 +12810,7 @@
         <v>5</v>
       </c>
       <c r="AD9">
-        <f t="shared" ref="AD9:AD10" si="0">(W9+Z9)/AC9*100</f>
+        <f t="shared" ref="AD9:AD10" si="4">(W9+Z9)/AC9*100</f>
         <v>100</v>
       </c>
       <c r="AF9">
@@ -12399,7 +12820,7 @@
         <v>5</v>
       </c>
       <c r="AH9">
-        <f>AG9/AI9*100</f>
+        <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
       <c r="AI9">
@@ -12412,14 +12833,14 @@
         <v>1</v>
       </c>
       <c r="AL9">
-        <f>AJ9/AK9*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="AM9">
         <v>6</v>
       </c>
       <c r="AN9">
-        <f>(AG9+AJ9)/AM9*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -12476,7 +12897,7 @@
         <v>0</v>
       </c>
       <c r="X10">
-        <f>W10/Y10*100</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Y10">
@@ -12489,14 +12910,14 @@
         <v>1</v>
       </c>
       <c r="AB10">
-        <f t="shared" ref="AB9:AB10" si="1">Z10/AA10*100</f>
+        <f t="shared" ref="AB10" si="5">Z10/AA10*100</f>
         <v>0</v>
       </c>
       <c r="AC10">
         <v>1</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AF10">
@@ -12506,7 +12927,7 @@
         <v>0</v>
       </c>
       <c r="AH10">
-        <f>AG10/AI10*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI10">
@@ -12519,14 +12940,14 @@
         <v>1</v>
       </c>
       <c r="AL10">
-        <f>AJ10/AK10*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="AM10">
         <v>1</v>
       </c>
       <c r="AN10">
-        <f>(AG10+AJ10)/AM10*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -12577,7 +12998,7 @@
         <v>0</v>
       </c>
       <c r="AH11">
-        <f>AG11/AI11*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI11">
@@ -12590,14 +13011,14 @@
         <v>1</v>
       </c>
       <c r="AL11">
-        <f>AJ11/AK11*100</f>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="AM11">
         <v>1</v>
       </c>
       <c r="AN11">
-        <f>(AG11+AJ11)/AM11*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -12654,7 +13075,7 @@
         <v>0</v>
       </c>
       <c r="AH12">
-        <f>AG12/AI12*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AI12">
@@ -12667,14 +13088,14 @@
         <v>1</v>
       </c>
       <c r="AL12">
-        <f>AJ12/AK12*100</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AM12">
         <v>1</v>
       </c>
       <c r="AN12">
-        <f>(AG12+AJ12)/AM12*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>